<commit_message>
travail sur les deplacement et la gravité en fct des fps
</commit_message>
<xml_diff>
--- a/Super_Retro_World_v2/Planning_2018_v1.xlsx
+++ b/Super_Retro_World_v2/Planning_2018_v1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
@@ -256,7 +256,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
   <si>
     <t>Débuter au</t>
   </si>
@@ -445,6 +445,9 @@
   </si>
   <si>
     <t>Lot physique générale</t>
+  </si>
+  <si>
+    <t>Déplacements</t>
   </si>
 </sst>
 </file>
@@ -15563,44 +15566,7 @@
     <cellStyle name="差_Suivi postes et candidats " xfId="3121"/>
     <cellStyle name="標準_CAR FLOW 2004 84 for A3 20040907 &amp; BUDGET B2005 " xfId="3122"/>
   </cellStyles>
-  <dxfs count="283">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="57">
     <dxf>
       <fill>
         <patternFill>
@@ -15611,362 +15577,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9AD8A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF42943C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF2C6129"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9AD8A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF42943C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF2C6129"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9AD8A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF42943C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF2C6129"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -16340,13 +15951,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="8" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
@@ -16374,1249 +15978,6 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9AD8A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF42943C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF2C6129"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9AD8A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF42943C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF2C6129"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9AD8A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF42943C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF2C6129"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9AD8A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF42943C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF2C6129"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9AD8A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF42943C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF2C6129"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9AD8A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF42943C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF2C6129"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9AD8A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF42943C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF2C6129"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9AD8A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF42943C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF2C6129"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9AD8A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF42943C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF2C6129"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -20647,7 +19008,7 @@
   <dimension ref="A1:GJ43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:F14"/>
+      <selection activeCell="E19" sqref="E19:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" outlineLevelRow="2"/>
@@ -29765,7 +28126,7 @@
       </c>
       <c r="E15" s="19">
         <f>MIN(E16:E19)</f>
-        <v>43235</v>
+        <v>43221</v>
       </c>
       <c r="F15" s="19">
         <f>MAX(F16:F19)</f>
@@ -29893,59 +28254,59 @@
       </c>
       <c r="AK15" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL15" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM15" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN15" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO15" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP15" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ15" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR15" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS15" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT15" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU15" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV15" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW15" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX15" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY15" s="21">
         <f t="shared" ca="1" si="16"/>
@@ -32773,10 +31134,14 @@
         <v>29</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="25"/>
+        <v>63</v>
+      </c>
+      <c r="E19" s="24">
+        <v>43221</v>
+      </c>
+      <c r="F19" s="25">
+        <v>43252</v>
+      </c>
       <c r="G19" s="20">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -32899,131 +31264,131 @@
       </c>
       <c r="AK19" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL19" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM19" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN19" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO19" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP19" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ19" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR19" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS19" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT19" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU19" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV19" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW19" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX19" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY19" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ19" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA19" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB19" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC19" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD19" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE19" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF19" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG19" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH19" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI19" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ19" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK19" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL19" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM19" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN19" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO19" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP19" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ19" s="21">
         <f t="shared" ca="1" si="17"/>
@@ -50247,282 +48612,282 @@
     <mergeCell ref="X2:AN2"/>
   </mergeCells>
   <conditionalFormatting sqref="G5:GG41">
-    <cfRule type="expression" dxfId="111" priority="56">
+    <cfRule type="expression" dxfId="56" priority="56">
       <formula>G$4=EOMONTH(G$4,-1)+1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:GG4">
-    <cfRule type="expression" dxfId="110" priority="55">
+    <cfRule type="expression" dxfId="55" priority="55">
       <formula>G$4=EOMONTH(G$4,-1)+1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:B5 D5:CK5 GD5:XFD5">
-    <cfRule type="cellIs" dxfId="109" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="54" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:B6 A11:B11 A15:B15 D15:CK15 D11:CK11 D6:CK6 GD15:XFD15 GD11:XFD11 GD6:XFD6 GD13:XFD13">
-    <cfRule type="cellIs" dxfId="108" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="53" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:B10 A12:B12 A16:B19 D12:CK12 D7:CK10 GD16:XFD19 GD12:XFD12 GD7:XFD10 GD14:XFD14 D16:CK19">
-    <cfRule type="cellIs" dxfId="107" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="52" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:B20 D20:CK20 GD20:XFD20">
-    <cfRule type="cellIs" dxfId="106" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="51" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:B21 D21:CK21 GD21:XFD21">
-    <cfRule type="cellIs" dxfId="105" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="50" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:B25 D22:CK25 GD22:XFD25">
-    <cfRule type="cellIs" dxfId="104" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="49" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B26 D26:CK26 GD26:XFD26">
-    <cfRule type="cellIs" dxfId="103" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="48" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:B27 D27:CK27 GD27:XFD27">
-    <cfRule type="cellIs" dxfId="102" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="47" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:B31 D28:CK31 GD28:XFD31">
-    <cfRule type="cellIs" dxfId="101" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="46" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32:B32 D32:CK32 GD32:XFD32">
-    <cfRule type="cellIs" dxfId="100" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="45" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33:B33 D33:CK33 GD33:XFD33">
-    <cfRule type="cellIs" dxfId="99" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="44" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:B37 D34:CK37 GD34:XFD37">
-    <cfRule type="cellIs" dxfId="98" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="43" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:B38 D38:CK38 GD38:XFD38">
-    <cfRule type="cellIs" dxfId="97" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="42" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:B39 D39:CK39 GD39:XFD39">
-    <cfRule type="cellIs" dxfId="96" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="41" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40:B41 D40:CK41 GD40:XFD41">
-    <cfRule type="cellIs" dxfId="95" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="40" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:B14 D14:CK14">
-    <cfRule type="cellIs" dxfId="94" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="38" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:B13 D13:CK13">
-    <cfRule type="cellIs" dxfId="93" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL14:GC14">
-    <cfRule type="cellIs" dxfId="92" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="21" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL5:GC5">
-    <cfRule type="cellIs" dxfId="91" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL15:GC15 CL11:GC11 CL6:GC6">
-    <cfRule type="cellIs" dxfId="90" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="36" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL16:GC19 CL12:GC12 CL7:GC10">
-    <cfRule type="cellIs" dxfId="89" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL20:GC20">
-    <cfRule type="cellIs" dxfId="88" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL21:GC21">
-    <cfRule type="cellIs" dxfId="87" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL22:GC25">
-    <cfRule type="cellIs" dxfId="86" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL26:GC26">
-    <cfRule type="cellIs" dxfId="85" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL27:GC27">
-    <cfRule type="cellIs" dxfId="84" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL28:GC31">
-    <cfRule type="cellIs" dxfId="83" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL32:GC32">
-    <cfRule type="cellIs" dxfId="82" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL33:GC33">
-    <cfRule type="cellIs" dxfId="81" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL34:GC37">
-    <cfRule type="cellIs" dxfId="80" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL38:GC38">
-    <cfRule type="cellIs" dxfId="79" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL39:GC39">
-    <cfRule type="cellIs" dxfId="78" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL40:GC41">
-    <cfRule type="cellIs" dxfId="77" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL13:GC13">
-    <cfRule type="cellIs" dxfId="76" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="75" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15 C11 C6">
-    <cfRule type="cellIs" dxfId="74" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:C19 C12 C7:C10">
-    <cfRule type="cellIs" dxfId="73" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="cellIs" dxfId="72" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="cellIs" dxfId="71" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C25">
-    <cfRule type="cellIs" dxfId="70" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="cellIs" dxfId="69" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="cellIs" dxfId="68" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C31">
-    <cfRule type="cellIs" dxfId="67" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="cellIs" dxfId="66" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="65" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:C37">
-    <cfRule type="cellIs" dxfId="64" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="cellIs" dxfId="63" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="cellIs" dxfId="62" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40:C41">
-    <cfRule type="cellIs" dxfId="61" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="60" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="59" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:GG41">
-    <cfRule type="expression" dxfId="58" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>G$4=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:GG3">
-    <cfRule type="expression" dxfId="57" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>G$4=EOMONTH(G$4,-1)+1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D41">
-    <cfRule type="expression" dxfId="56" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>AND($E5&lt;=TODAY(),$F5&gt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>